<commit_message>
Audios sistemas generativos recortados
</commit_message>
<xml_diff>
--- a/audios_eval_sist_generativos/Checklist_Prompts_Sistemas.xlsx
+++ b/audios_eval_sist_generativos/Checklist_Prompts_Sistemas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Escritorio\I2ADE\5º I2ADE\TRABAJOS DE FIN DE GRADO\TFG INFORMÁTICA\TFG EVALUACIÓN Y RED NEURONAL\tfg-informatica-IA\audios_eval_sist_generativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CE5667-1FCE-4E13-9B0E-5884CC839F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD9601B-391D-49FB-AB6D-21AF89D603FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="32">
   <si>
     <t>Género</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Classical</t>
   </si>
   <si>
-    <t>Disco</t>
-  </si>
-  <si>
     <t>Metal</t>
   </si>
   <si>
@@ -69,21 +66,6 @@
     <t>Generate a 30-second classical piece that feels calm and peaceful.</t>
   </si>
   <si>
-    <t>Generate a 30-second disco music song.</t>
-  </si>
-  <si>
-    <t>Generate a 30-second instrumental disco music groove.</t>
-  </si>
-  <si>
-    <t>Generate a 30-second 70s disco song inspired by Donna Summer.</t>
-  </si>
-  <si>
-    <t>Generate a 30-second nu-disco song inspired by Daft Punk.</t>
-  </si>
-  <si>
-    <t>Generate a 30-second disco piece that feels energetic and fun.</t>
-  </si>
-  <si>
     <t>Generate a 30-second metal music song.</t>
   </si>
   <si>
@@ -118,6 +100,24 @@
   </si>
   <si>
     <t>Se usan estilos predeterminados parecidos como semilla</t>
+  </si>
+  <si>
+    <t>Generate a 30-second jazz music song.</t>
+  </si>
+  <si>
+    <t>Generate a 30-second jazz instrumental piece.</t>
+  </si>
+  <si>
+    <t>Generate a 30-second bebop jazz piece inspired by Charlie Parker.</t>
+  </si>
+  <si>
+    <t>Generate a 30-second swing jazz song in the style of Duke Ellington.</t>
+  </si>
+  <si>
+    <t>Jazz</t>
+  </si>
+  <si>
+    <t>Generate a 30-second jazz song that sounds melancholic and nostalgic.</t>
   </si>
 </sst>
 </file>
@@ -215,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -225,14 +225,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -542,7 +539,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,11 +565,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>29</v>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -580,13 +577,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -598,13 +595,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -616,13 +613,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -634,13 +631,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -652,13 +649,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
         <v>1</v>
@@ -667,86 +664,106 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -755,16 +772,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -773,16 +790,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -791,16 +808,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2">
         <v>1</v>
@@ -809,16 +826,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -835,7 +852,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,10 +879,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -873,19 +890,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -893,19 +910,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -913,19 +930,19 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -933,19 +950,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -953,189 +970,219 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1195,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,10 +1222,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>29</v>
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1186,13 +1233,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1204,13 +1251,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1222,13 +1269,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1240,13 +1287,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1258,13 +1305,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -1273,86 +1320,106 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -1361,16 +1428,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
@@ -1379,42 +1446,42 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>30</v>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -1423,16 +1490,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>

</xml_diff>